<commit_message>
Ajuste do conteúdo da célula
</commit_message>
<xml_diff>
--- a/Notas.xlsx
+++ b/Notas.xlsx
@@ -16,7 +16,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <name val="Calibri"/>
@@ -46,8 +48,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -420,6 +423,13 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="36" customWidth="1" min="1" max="1"/>
+    <col width="5" customWidth="1" min="2" max="2"/>
+    <col width="5" customWidth="1" min="3" max="3"/>
+    <col width="5" customWidth="1" min="4" max="4"/>
+    <col width="13" customWidth="1" min="5" max="5"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -454,25 +464,17 @@
           <t>Física</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="B2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -481,25 +483,17 @@
           <t>Poo</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="B3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -508,25 +502,17 @@
           <t>Inglês</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="B4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -535,25 +521,17 @@
           <t>Extensão</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="B5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -562,25 +540,17 @@
           <t>Algoritimos e estrutura de dados</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="B6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -589,25 +559,17 @@
           <t>Fundamentos de Fabricação</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="B7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -616,25 +578,17 @@
           <t>Sistemas Hidráulicos e pneumáticos</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="B8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>